<commit_message>
Update Sprint 2 burndownchart.xlsx
</commit_message>
<xml_diff>
--- a/Sprint 2 burndownchart.xlsx
+++ b/Sprint 2 burndownchart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\trophyHoardGame\Trophy-Hoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph Earl\Desktop\New folder\Trophy-Hoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6B9E5B-CE07-4315-B715-8AF5B869149E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BE46A7-4798-471C-B715-636AD7B9A3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{880ECEA2-B438-484A-9CBA-91374F2777E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{880ECEA2-B438-484A-9CBA-91374F2777E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Iteration" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -183,13 +194,13 @@
     <t>Animations</t>
   </si>
   <si>
-    <t>Models</t>
-  </si>
-  <si>
     <t>Main Menu</t>
   </si>
   <si>
     <t>Gameplay UI</t>
+  </si>
+  <si>
+    <t>Dungeon Level Design</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1030,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>83</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -1152,37 +1163,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>83</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.7</c:v>
+                  <c:v>128.69999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66.400000000000006</c:v>
+                  <c:v>114.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.100000000000009</c:v>
+                  <c:v>100.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.800000000000011</c:v>
+                  <c:v>85.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.500000000000014</c:v>
+                  <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.200000000000017</c:v>
+                  <c:v>57.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.900000000000016</c:v>
+                  <c:v>42.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.600000000000016</c:v>
+                  <c:v>28.600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.3000000000000149</c:v>
+                  <c:v>14.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.4210854715202004E-14</c:v>
+                  <c:v>3.5527136788005009E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1629,7 +1640,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>83</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -1811,37 +1822,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>83</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.7</c:v>
+                  <c:v>128.69999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66.400000000000006</c:v>
+                  <c:v>114.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.100000000000009</c:v>
+                  <c:v>100.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.800000000000011</c:v>
+                  <c:v>85.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.500000000000014</c:v>
+                  <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.200000000000017</c:v>
+                  <c:v>57.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.900000000000016</c:v>
+                  <c:v>42.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.600000000000016</c:v>
+                  <c:v>28.600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.3000000000000149</c:v>
+                  <c:v>14.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.4210854715202004E-14</c:v>
+                  <c:v>3.5527136788005009E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3656,19 +3667,19 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
+      <selection pane="bottomRight" activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="22" width="5.7109375" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="12" width="5.6640625" customWidth="1"/>
+    <col min="13" max="22" width="5.6640625" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="37"/>
       <c r="B1" s="37"/>
       <c r="C1" s="6"/>
@@ -3694,7 +3705,7 @@
       <c r="W1" s="15"/>
       <c r="X1" s="16"/>
     </row>
-    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="40" t="s">
@@ -3724,7 +3735,7 @@
       <c r="W2" s="15"/>
       <c r="X2" s="16"/>
     </row>
-    <row r="3" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="40" t="s">
@@ -3735,7 +3746,7 @@
       <c r="F3" s="40"/>
       <c r="G3" s="33">
         <f>B38</f>
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
@@ -3755,7 +3766,7 @@
       <c r="W3" s="15"/>
       <c r="X3" s="16"/>
     </row>
-    <row r="4" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="40" t="s">
@@ -3785,7 +3796,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="16"/>
     </row>
-    <row r="5" spans="1:24" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="97.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="34" t="s">
         <v>0</v>
       </c>
@@ -3813,7 +3824,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="16"/>
     </row>
-    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="39" t="s">
         <v>1</v>
       </c>
@@ -3845,7 +3856,7 @@
       </c>
       <c r="X6" s="42"/>
     </row>
-    <row r="7" spans="1:24" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -3919,7 +3930,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -3955,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
@@ -3977,11 +3988,21 @@
       <c r="G9" s="22">
         <v>4.5</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="23"/>
+      <c r="H9" s="23">
+        <v>0</v>
+      </c>
+      <c r="I9" s="22">
+        <v>0</v>
+      </c>
+      <c r="J9" s="23">
+        <v>0</v>
+      </c>
+      <c r="K9" s="22">
+        <v>0</v>
+      </c>
+      <c r="L9" s="23">
+        <v>0</v>
+      </c>
       <c r="M9" s="22"/>
       <c r="N9" s="23"/>
       <c r="O9" s="22"/>
@@ -4001,12 +4022,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B10" s="21">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C10" s="22">
         <v>0</v>
@@ -4023,11 +4044,21 @@
       <c r="G10" s="22">
         <v>0</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="23"/>
+      <c r="H10" s="23">
+        <v>13</v>
+      </c>
+      <c r="I10" s="22">
+        <v>6</v>
+      </c>
+      <c r="J10" s="23">
+        <v>3</v>
+      </c>
+      <c r="K10" s="22">
+        <v>4.5</v>
+      </c>
+      <c r="L10" s="23">
+        <v>5</v>
+      </c>
       <c r="M10" s="22"/>
       <c r="N10" s="23"/>
       <c r="O10" s="22"/>
@@ -4040,16 +4071,16 @@
       <c r="V10" s="23"/>
       <c r="W10" s="28">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>48.5</v>
       </c>
       <c r="X10" s="17">
         <f t="shared" ref="X10:X38" si="1">IFERROR(1-(W10/B10),"")</f>
-        <v>0</v>
+        <v>0.39375000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="21">
         <v>12</v>
@@ -4103,9 +4134,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="21">
         <v>14</v>
@@ -4159,7 +4190,7 @@
         <v>0.85714285714285721</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -4193,7 +4224,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -4227,7 +4258,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -4261,7 +4292,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -4295,7 +4326,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -4329,7 +4360,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
@@ -4363,7 +4394,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -4397,7 +4428,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>10</v>
       </c>
@@ -4431,7 +4462,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>11</v>
       </c>
@@ -4465,7 +4496,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>12</v>
       </c>
@@ -4499,7 +4530,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
@@ -4533,7 +4564,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>14</v>
       </c>
@@ -4567,7 +4598,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -4601,7 +4632,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -4635,7 +4666,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -4669,7 +4700,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
@@ -4703,7 +4734,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -4737,7 +4768,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>20</v>
       </c>
@@ -4771,7 +4802,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>21</v>
       </c>
@@ -4805,7 +4836,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
@@ -4839,7 +4870,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
@@ -4873,7 +4904,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
         <v>24</v>
       </c>
@@ -4907,7 +4938,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
         <v>25</v>
       </c>
@@ -4941,7 +4972,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
         <v>26</v>
       </c>
@@ -4975,7 +5006,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>27</v>
       </c>
@@ -5009,13 +5040,13 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A38" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B38" s="10">
         <f>SUM(B8:B37)</f>
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="C38" s="11" t="e">
         <f>IFERROR(IF(B38-SUM(C8:C37)=B38,NA(),B38-SUM(C8:C37)),NA())</f>
@@ -5099,60 +5130,60 @@
       </c>
       <c r="W38" s="35">
         <f>SUM(W8:W37)</f>
-        <v>45.5</v>
+        <v>74</v>
       </c>
       <c r="X38" s="30">
         <f t="shared" si="1"/>
-        <v>0.45180722891566261</v>
+        <v>0.4825174825174825</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B39" s="12">
         <f>SUM(B8:B37)</f>
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="C39" s="13">
         <f>IFERROR((IF(B39-($B$38/$G$4) &lt; 0,"-", B39-($B$38/$G$4))),IFERROR(B39-($B$38/20),"-"))</f>
-        <v>74.7</v>
+        <v>128.69999999999999</v>
       </c>
       <c r="D39" s="13">
         <f t="shared" ref="D39:V39" si="3">IFERROR((IF(C39-($B$38/$G$4) &lt; 0,"-", C39-($B$38/$G$4))),IFERROR(C39-($B$38/20),"-"))</f>
-        <v>66.400000000000006</v>
+        <v>114.39999999999999</v>
       </c>
       <c r="E39" s="13">
         <f t="shared" si="3"/>
-        <v>58.100000000000009</v>
+        <v>100.1</v>
       </c>
       <c r="F39" s="13">
         <f t="shared" si="3"/>
-        <v>49.800000000000011</v>
+        <v>85.8</v>
       </c>
       <c r="G39" s="13">
         <f t="shared" si="3"/>
-        <v>41.500000000000014</v>
+        <v>71.5</v>
       </c>
       <c r="H39" s="13">
         <f t="shared" si="3"/>
-        <v>33.200000000000017</v>
+        <v>57.2</v>
       </c>
       <c r="I39" s="13">
         <f t="shared" si="3"/>
-        <v>24.900000000000016</v>
+        <v>42.900000000000006</v>
       </c>
       <c r="J39" s="13">
         <f t="shared" si="3"/>
-        <v>16.600000000000016</v>
+        <v>28.600000000000005</v>
       </c>
       <c r="K39" s="13">
         <f t="shared" si="3"/>
-        <v>8.3000000000000149</v>
+        <v>14.300000000000004</v>
       </c>
       <c r="L39" s="13">
         <f t="shared" si="3"/>
-        <v>1.4210854715202004E-14</v>
+        <v>3.5527136788005009E-15</v>
       </c>
       <c r="M39" s="13" t="str">
         <f t="shared" si="3"/>
@@ -5197,7 +5228,7 @@
       <c r="W39" s="31"/>
       <c r="X39" s="32"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A1:B2"/>
@@ -5261,7 +5292,7 @@
       <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>